<commit_message>
update with excel data driven
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2023SepWorkSpace\ERPAutomation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2024_LiveProjects\LiveProject_Cucumber\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F91C27-995A-476D-846B-C19DAC1A4993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="1" r:id="rId1"/>
-    <sheet name="dataSheet" sheetId="2" r:id="rId2"/>
-    <sheet name="Categories" sheetId="3" r:id="rId3"/>
-    <sheet name="UOM" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="dataSheet" sheetId="2" r:id="rId3"/>
+    <sheet name="Categories" sheetId="3" r:id="rId4"/>
+    <sheet name="UOM" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -110,7 +112,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -170,7 +172,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1"/>
@@ -180,7 +182,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -462,11 +463,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD5"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,19 +501,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Secret@123"/>
-    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1" display="Secret@123" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDA6981-A4A0-46FD-A5D5-FE0A3B192023}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,8 +591,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -595,17 +610,17 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -614,11 +629,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>

</xml_diff>